<commit_message>
fix test_input file excel
</commit_message>
<xml_diff>
--- a/Test_input.xlsx
+++ b/Test_input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nguye\OneDrive\Máy tính\Web_KTPM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C5888DD-79DB-42FD-9D09-5A4F7E5B99CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FCFE333-E94D-4DC1-8EFB-8BB26FC5A577}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5F1CD735-948A-4F17-A1DF-359A80976EDA}"/>
   </bookViews>
@@ -422,11 +422,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -434,11 +437,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -781,8 +781,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7B3A9CF-6CB7-420E-992E-F2960A782706}">
   <dimension ref="A1:F130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G121" sqref="G121"/>
+    <sheetView tabSelected="1" topLeftCell="B96" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H128" sqref="H128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -794,43 +794,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="11" t="s">
+      <c r="C2" s="11"/>
+      <c r="D2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="10" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="9"/>
+      <c r="A3" s="11"/>
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="11"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="14"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="10"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
@@ -848,7 +848,7 @@
       <c r="E4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="F4" s="9" t="s">
         <v>88</v>
       </c>
     </row>
@@ -868,7 +868,7 @@
       <c r="E5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="F5" s="9" t="s">
         <v>88</v>
       </c>
     </row>
@@ -888,7 +888,7 @@
       <c r="E6" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="13" t="s">
+      <c r="F6" s="9" t="s">
         <v>88</v>
       </c>
     </row>
@@ -908,7 +908,7 @@
       <c r="E7" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="13" t="s">
+      <c r="F7" s="9" t="s">
         <v>88</v>
       </c>
     </row>
@@ -928,7 +928,7 @@
       <c r="E8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="13" t="s">
+      <c r="F8" s="9" t="s">
         <v>88</v>
       </c>
     </row>
@@ -948,7 +948,7 @@
       <c r="E9" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="13" t="s">
+      <c r="F9" s="9" t="s">
         <v>88</v>
       </c>
     </row>
@@ -968,48 +968,48 @@
       <c r="E10" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F10" s="13" t="s">
+      <c r="F10" s="9" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C13" s="9"/>
-      <c r="D13" s="11" t="s">
+      <c r="C13" s="11"/>
+      <c r="D13" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="E13" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F13" s="14" t="s">
+      <c r="F13" s="10" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="9"/>
+      <c r="A14" s="11"/>
       <c r="B14" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D14" s="11"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="14"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="10"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
@@ -1027,7 +1027,7 @@
       <c r="E15" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F15" s="13" t="s">
+      <c r="F15" s="9" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1047,48 +1047,48 @@
       <c r="E16" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F16" s="13" t="s">
+      <c r="F16" s="9" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="10" t="s">
+      <c r="A18" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="9" t="s">
+      <c r="A19" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C19" s="9"/>
-      <c r="D19" s="11" t="s">
+      <c r="C19" s="11"/>
+      <c r="D19" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E19" s="9" t="s">
+      <c r="E19" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F19" s="14" t="s">
+      <c r="F19" s="10" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="9"/>
+      <c r="A20" s="11"/>
       <c r="B20" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D20" s="11"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="14"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="10"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
@@ -1106,7 +1106,7 @@
       <c r="E21" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F21" s="13" t="s">
+      <c r="F21" s="9" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1126,48 +1126,48 @@
       <c r="E22" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F22" s="13" t="s">
+      <c r="F22" s="9" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="10" t="s">
+      <c r="A24" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="B24" s="10"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="9" t="s">
+      <c r="A25" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B25" s="9" t="s">
+      <c r="B25" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C25" s="9"/>
-      <c r="D25" s="11" t="s">
+      <c r="C25" s="11"/>
+      <c r="D25" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E25" s="9" t="s">
+      <c r="E25" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F25" s="14" t="s">
+      <c r="F25" s="10" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="9"/>
+      <c r="A26" s="11"/>
       <c r="B26" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D26" s="11"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="14"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="10"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
@@ -1185,7 +1185,7 @@
       <c r="E27" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F27" s="13" t="s">
+      <c r="F27" s="9" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1205,7 +1205,7 @@
       <c r="E28" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F28" s="13" t="s">
+      <c r="F28" s="9" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1225,7 +1225,7 @@
       <c r="E29" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F29" s="13" t="s">
+      <c r="F29" s="9" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1245,7 +1245,7 @@
       <c r="E30" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F30" s="13" t="s">
+      <c r="F30" s="9" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1265,7 +1265,7 @@
       <c r="E31" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F31" s="13" t="s">
+      <c r="F31" s="9" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1285,7 +1285,7 @@
       <c r="E32" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F32" s="13" t="s">
+      <c r="F32" s="9" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1305,44 +1305,44 @@
       <c r="E33" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F33" s="13" t="s">
+      <c r="F33" s="9" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A35" s="12" t="s">
+      <c r="A35" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B35" s="12"/>
-      <c r="C35" s="12"/>
-      <c r="D35" s="12"/>
+      <c r="B35" s="13"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
       <c r="E35" s="4"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36" s="9" t="s">
+      <c r="A36" s="11" t="s">
         <v>0</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C36" s="11" t="s">
+      <c r="C36" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D36" s="9" t="s">
+      <c r="D36" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F36" s="14" t="s">
+      <c r="F36" s="10" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A37" s="9"/>
+      <c r="A37" s="11"/>
       <c r="B37" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C37" s="11"/>
-      <c r="D37" s="9"/>
-      <c r="F37" s="14"/>
+      <c r="C37" s="12"/>
+      <c r="D37" s="11"/>
+      <c r="F37" s="10"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
@@ -1357,7 +1357,7 @@
       <c r="D38" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="F38" s="13" t="s">
+      <c r="F38" s="9" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1374,44 +1374,44 @@
       <c r="D39" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F39" s="13" t="s">
+      <c r="F39" s="9" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A41" s="12" t="s">
+      <c r="A41" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B41" s="12"/>
-      <c r="C41" s="12"/>
-      <c r="D41" s="12"/>
+      <c r="B41" s="13"/>
+      <c r="C41" s="13"/>
+      <c r="D41" s="13"/>
       <c r="E41" s="4"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A42" s="9" t="s">
+      <c r="A42" s="11" t="s">
         <v>5</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C42" s="11" t="s">
+      <c r="C42" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D42" s="9" t="s">
+      <c r="D42" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F42" s="14" t="s">
+      <c r="F42" s="10" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A43" s="9"/>
+      <c r="A43" s="11"/>
       <c r="B43" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C43" s="11"/>
-      <c r="D43" s="9"/>
-      <c r="F43" s="14"/>
+      <c r="C43" s="12"/>
+      <c r="D43" s="11"/>
+      <c r="F43" s="10"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
@@ -1426,7 +1426,7 @@
       <c r="D44" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F44" s="13" t="s">
+      <c r="F44" s="9" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1443,7 +1443,7 @@
       <c r="D45" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="F45" s="13" t="s">
+      <c r="F45" s="9" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1460,7 +1460,7 @@
       <c r="D46" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F46" s="13" t="s">
+      <c r="F46" s="9" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1477,7 +1477,7 @@
       <c r="D47" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="F47" s="13" t="s">
+      <c r="F47" s="9" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1494,7 +1494,7 @@
       <c r="D48" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F48" s="13" t="s">
+      <c r="F48" s="9" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1509,43 +1509,43 @@
       <c r="D49" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="F49" s="13" t="s">
+      <c r="F49" s="9" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A51" s="12" t="s">
+      <c r="A51" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="B51" s="12"/>
-      <c r="C51" s="12"/>
-      <c r="D51" s="12"/>
+      <c r="B51" s="13"/>
+      <c r="C51" s="13"/>
+      <c r="D51" s="13"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A52" s="9" t="s">
+      <c r="A52" s="11" t="s">
         <v>0</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C52" s="11" t="s">
+      <c r="C52" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D52" s="9" t="s">
+      <c r="D52" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F52" s="14" t="s">
+      <c r="F52" s="10" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A53" s="9"/>
+      <c r="A53" s="11"/>
       <c r="B53" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C53" s="11"/>
-      <c r="D53" s="9"/>
-      <c r="F53" s="14"/>
+      <c r="C53" s="12"/>
+      <c r="D53" s="11"/>
+      <c r="F53" s="10"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
@@ -1560,7 +1560,7 @@
       <c r="D54" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="F54" s="13" t="s">
+      <c r="F54" s="9" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1577,43 +1577,43 @@
       <c r="D55" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F55" s="13" t="s">
+      <c r="F55" s="9" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A57" s="12" t="s">
+      <c r="A57" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="B57" s="12"/>
-      <c r="C57" s="12"/>
-      <c r="D57" s="12"/>
+      <c r="B57" s="13"/>
+      <c r="C57" s="13"/>
+      <c r="D57" s="13"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A58" s="9" t="s">
+      <c r="A58" s="11" t="s">
         <v>5</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C58" s="11" t="s">
+      <c r="C58" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D58" s="9" t="s">
+      <c r="D58" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F58" s="14" t="s">
+      <c r="F58" s="10" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A59" s="9"/>
+      <c r="A59" s="11"/>
       <c r="B59" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C59" s="11"/>
-      <c r="D59" s="9"/>
-      <c r="F59" s="14"/>
+      <c r="C59" s="12"/>
+      <c r="D59" s="11"/>
+      <c r="F59" s="10"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
@@ -1628,7 +1628,7 @@
       <c r="D60" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F60" s="13" t="s">
+      <c r="F60" s="9" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1645,7 +1645,7 @@
       <c r="D61" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="F61" s="13" t="s">
+      <c r="F61" s="9" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1662,7 +1662,7 @@
       <c r="D62" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="F62" s="13" t="s">
+      <c r="F62" s="9" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1679,48 +1679,48 @@
       <c r="D63" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F63" s="13" t="s">
+      <c r="F63" s="9" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A65" s="10" t="s">
+      <c r="A65" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="B65" s="10"/>
-      <c r="C65" s="10"/>
-      <c r="D65" s="10"/>
-      <c r="E65" s="10"/>
+      <c r="B65" s="14"/>
+      <c r="C65" s="14"/>
+      <c r="D65" s="14"/>
+      <c r="E65" s="14"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A66" s="9" t="s">
+      <c r="A66" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B66" s="9" t="s">
+      <c r="B66" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C66" s="9"/>
-      <c r="D66" s="11" t="s">
+      <c r="C66" s="11"/>
+      <c r="D66" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E66" s="9" t="s">
+      <c r="E66" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F66" s="14" t="s">
+      <c r="F66" s="10" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A67" s="9"/>
+      <c r="A67" s="11"/>
       <c r="B67" s="2" t="s">
         <v>57</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D67" s="11"/>
-      <c r="E67" s="9"/>
-      <c r="F67" s="14"/>
+      <c r="D67" s="12"/>
+      <c r="E67" s="11"/>
+      <c r="F67" s="10"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" s="3" t="s">
@@ -1738,7 +1738,7 @@
       <c r="E68" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="F68" s="13" t="s">
+      <c r="F68" s="9" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1758,48 +1758,48 @@
       <c r="E69" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="F69" s="13" t="s">
+      <c r="F69" s="9" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A71" s="10" t="s">
+      <c r="A71" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="B71" s="10"/>
-      <c r="C71" s="10"/>
-      <c r="D71" s="10"/>
-      <c r="E71" s="10"/>
+      <c r="B71" s="14"/>
+      <c r="C71" s="14"/>
+      <c r="D71" s="14"/>
+      <c r="E71" s="14"/>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A72" s="9" t="s">
+      <c r="A72" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B72" s="9" t="s">
+      <c r="B72" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C72" s="9"/>
-      <c r="D72" s="11" t="s">
+      <c r="C72" s="11"/>
+      <c r="D72" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E72" s="9" t="s">
+      <c r="E72" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F72" s="14" t="s">
+      <c r="F72" s="10" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A73" s="9"/>
+      <c r="A73" s="11"/>
       <c r="B73" s="2" t="s">
         <v>57</v>
       </c>
       <c r="C73" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D73" s="11"/>
-      <c r="E73" s="9"/>
-      <c r="F73" s="14"/>
+      <c r="D73" s="12"/>
+      <c r="E73" s="11"/>
+      <c r="F73" s="10"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" s="3" t="s">
@@ -1817,7 +1817,7 @@
       <c r="E74" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="F74" s="13" t="s">
+      <c r="F74" s="9" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1837,48 +1837,48 @@
       <c r="E75" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="F75" s="13" t="s">
+      <c r="F75" s="9" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A77" s="10" t="s">
+      <c r="A77" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="B77" s="10"/>
-      <c r="C77" s="10"/>
-      <c r="D77" s="10"/>
-      <c r="E77" s="10"/>
+      <c r="B77" s="14"/>
+      <c r="C77" s="14"/>
+      <c r="D77" s="14"/>
+      <c r="E77" s="14"/>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A78" s="9" t="s">
+      <c r="A78" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B78" s="9" t="s">
+      <c r="B78" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C78" s="9"/>
-      <c r="D78" s="11" t="s">
+      <c r="C78" s="11"/>
+      <c r="D78" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E78" s="9" t="s">
+      <c r="E78" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F78" s="14" t="s">
+      <c r="F78" s="10" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A79" s="9"/>
+      <c r="A79" s="11"/>
       <c r="B79" s="2" t="s">
         <v>57</v>
       </c>
       <c r="C79" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D79" s="11"/>
-      <c r="E79" s="9"/>
-      <c r="F79" s="14"/>
+      <c r="D79" s="12"/>
+      <c r="E79" s="11"/>
+      <c r="F79" s="10"/>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" s="3" t="s">
@@ -1896,7 +1896,7 @@
       <c r="E80" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="F80" s="13" t="s">
+      <c r="F80" s="9" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1916,48 +1916,48 @@
       <c r="E81" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="F81" s="13" t="s">
+      <c r="F81" s="9" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A83" s="10" t="s">
+      <c r="A83" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="B83" s="10"/>
-      <c r="C83" s="10"/>
-      <c r="D83" s="10"/>
-      <c r="E83" s="10"/>
+      <c r="B83" s="14"/>
+      <c r="C83" s="14"/>
+      <c r="D83" s="14"/>
+      <c r="E83" s="14"/>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A84" s="9" t="s">
+      <c r="A84" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B84" s="9" t="s">
+      <c r="B84" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C84" s="9"/>
-      <c r="D84" s="11" t="s">
+      <c r="C84" s="11"/>
+      <c r="D84" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E84" s="9" t="s">
+      <c r="E84" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F84" s="14" t="s">
+      <c r="F84" s="10" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A85" s="9"/>
+      <c r="A85" s="11"/>
       <c r="B85" s="2" t="s">
         <v>57</v>
       </c>
       <c r="C85" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D85" s="11"/>
-      <c r="E85" s="9"/>
-      <c r="F85" s="14"/>
+      <c r="D85" s="12"/>
+      <c r="E85" s="11"/>
+      <c r="F85" s="10"/>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86" s="3" t="s">
@@ -1975,7 +1975,7 @@
       <c r="E86" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="F86" s="13" t="s">
+      <c r="F86" s="9" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1995,7 +1995,7 @@
       <c r="E87" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="F87" s="13" t="s">
+      <c r="F87" s="9" t="s">
         <v>88</v>
       </c>
     </row>
@@ -2007,38 +2007,38 @@
       <c r="E88" s="3"/>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A90" s="12" t="s">
+      <c r="A90" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="B90" s="12"/>
-      <c r="C90" s="12"/>
-      <c r="D90" s="12"/>
+      <c r="B90" s="13"/>
+      <c r="C90" s="13"/>
+      <c r="D90" s="13"/>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A91" s="9" t="s">
+      <c r="A91" s="11" t="s">
         <v>0</v>
       </c>
       <c r="B91" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C91" s="11" t="s">
+      <c r="C91" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D91" s="9" t="s">
+      <c r="D91" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F91" s="14" t="s">
+      <c r="F91" s="10" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A92" s="9"/>
+      <c r="A92" s="11"/>
       <c r="B92" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C92" s="11"/>
-      <c r="D92" s="9"/>
-      <c r="F92" s="14"/>
+      <c r="C92" s="12"/>
+      <c r="D92" s="11"/>
+      <c r="F92" s="10"/>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93" s="3" t="s">
@@ -2053,7 +2053,7 @@
       <c r="D93" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="F93" s="13" t="s">
+      <c r="F93" s="9" t="s">
         <v>88</v>
       </c>
     </row>
@@ -2070,43 +2070,43 @@
       <c r="D94" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="F94" s="13" t="s">
+      <c r="F94" s="9" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A96" s="12" t="s">
+      <c r="A96" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="B96" s="12"/>
-      <c r="C96" s="12"/>
-      <c r="D96" s="12"/>
+      <c r="B96" s="13"/>
+      <c r="C96" s="13"/>
+      <c r="D96" s="13"/>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A97" s="9" t="s">
+      <c r="A97" s="11" t="s">
         <v>5</v>
       </c>
       <c r="B97" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C97" s="11" t="s">
+      <c r="C97" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D97" s="9" t="s">
+      <c r="D97" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F97" s="14" t="s">
+      <c r="F97" s="10" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A98" s="9"/>
+      <c r="A98" s="11"/>
       <c r="B98" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C98" s="11"/>
-      <c r="D98" s="9"/>
-      <c r="F98" s="14"/>
+      <c r="C98" s="12"/>
+      <c r="D98" s="11"/>
+      <c r="F98" s="10"/>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A99" s="3" t="s">
@@ -2121,7 +2121,7 @@
       <c r="D99" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="F99" s="13" t="s">
+      <c r="F99" s="9" t="s">
         <v>88</v>
       </c>
     </row>
@@ -2138,7 +2138,7 @@
       <c r="D100" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="F100" s="13" t="s">
+      <c r="F100" s="9" t="s">
         <v>88</v>
       </c>
     </row>
@@ -2155,7 +2155,7 @@
       <c r="D101" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="F101" s="13" t="s">
+      <c r="F101" s="9" t="s">
         <v>88</v>
       </c>
     </row>
@@ -2172,43 +2172,43 @@
       <c r="D102" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="F102" s="13" t="s">
+      <c r="F102" s="9" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A104" s="12" t="s">
+      <c r="A104" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="B104" s="12"/>
-      <c r="C104" s="12"/>
-      <c r="D104" s="12"/>
+      <c r="B104" s="13"/>
+      <c r="C104" s="13"/>
+      <c r="D104" s="13"/>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A105" s="9" t="s">
+      <c r="A105" s="11" t="s">
         <v>0</v>
       </c>
       <c r="B105" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C105" s="11" t="s">
+      <c r="C105" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D105" s="9" t="s">
+      <c r="D105" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F105" s="14" t="s">
+      <c r="F105" s="10" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A106" s="9"/>
+      <c r="A106" s="11"/>
       <c r="B106" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C106" s="11"/>
-      <c r="D106" s="9"/>
-      <c r="F106" s="14"/>
+      <c r="C106" s="12"/>
+      <c r="D106" s="11"/>
+      <c r="F106" s="10"/>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A107" s="3" t="s">
@@ -2223,7 +2223,7 @@
       <c r="D107" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="F107" s="13" t="s">
+      <c r="F107" s="9" t="s">
         <v>88</v>
       </c>
     </row>
@@ -2240,43 +2240,43 @@
       <c r="D108" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="F108" s="13" t="s">
+      <c r="F108" s="9" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A110" s="12" t="s">
+      <c r="A110" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="B110" s="12"/>
-      <c r="C110" s="12"/>
-      <c r="D110" s="12"/>
+      <c r="B110" s="13"/>
+      <c r="C110" s="13"/>
+      <c r="D110" s="13"/>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A111" s="9" t="s">
+      <c r="A111" s="11" t="s">
         <v>5</v>
       </c>
       <c r="B111" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C111" s="11" t="s">
+      <c r="C111" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D111" s="9" t="s">
+      <c r="D111" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F111" s="14" t="s">
+      <c r="F111" s="10" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A112" s="9"/>
+      <c r="A112" s="11"/>
       <c r="B112" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C112" s="11"/>
-      <c r="D112" s="9"/>
-      <c r="F112" s="14"/>
+      <c r="C112" s="12"/>
+      <c r="D112" s="11"/>
+      <c r="F112" s="10"/>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A113" s="3" t="s">
@@ -2291,7 +2291,7 @@
       <c r="D113" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="F113" s="13" t="s">
+      <c r="F113" s="9" t="s">
         <v>88</v>
       </c>
     </row>
@@ -2308,7 +2308,7 @@
       <c r="D114" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="F114" s="13" t="s">
+      <c r="F114" s="9" t="s">
         <v>88</v>
       </c>
     </row>
@@ -2325,43 +2325,43 @@
       <c r="D116" s="3"/>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A118" s="10" t="s">
+      <c r="A118" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="B118" s="10"/>
-      <c r="C118" s="10"/>
-      <c r="D118" s="10"/>
-      <c r="E118" s="10"/>
+      <c r="B118" s="14"/>
+      <c r="C118" s="14"/>
+      <c r="D118" s="14"/>
+      <c r="E118" s="14"/>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A119" s="9" t="s">
+      <c r="A119" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B119" s="9" t="s">
+      <c r="B119" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C119" s="9"/>
-      <c r="D119" s="11" t="s">
+      <c r="C119" s="11"/>
+      <c r="D119" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E119" s="9" t="s">
+      <c r="E119" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F119" s="14" t="s">
+      <c r="F119" s="10" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A120" s="9"/>
+      <c r="A120" s="11"/>
       <c r="B120" s="2" t="s">
         <v>81</v>
       </c>
       <c r="C120" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D120" s="11"/>
-      <c r="E120" s="9"/>
-      <c r="F120" s="14"/>
+      <c r="D120" s="12"/>
+      <c r="E120" s="11"/>
+      <c r="F120" s="10"/>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A121" s="3" t="s">
@@ -2379,7 +2379,7 @@
       <c r="E121" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="F121" s="13" t="s">
+      <c r="F121" s="9" t="s">
         <v>88</v>
       </c>
     </row>
@@ -2399,48 +2399,48 @@
       <c r="E122" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="F122" s="13" t="s">
+      <c r="F122" s="9" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A124" s="10" t="s">
+      <c r="A124" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="B124" s="10"/>
-      <c r="C124" s="10"/>
-      <c r="D124" s="10"/>
-      <c r="E124" s="10"/>
+      <c r="B124" s="14"/>
+      <c r="C124" s="14"/>
+      <c r="D124" s="14"/>
+      <c r="E124" s="14"/>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A125" s="9" t="s">
+      <c r="A125" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B125" s="9" t="s">
+      <c r="B125" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C125" s="9"/>
-      <c r="D125" s="11" t="s">
+      <c r="C125" s="11"/>
+      <c r="D125" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E125" s="9" t="s">
+      <c r="E125" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F125" s="14" t="s">
+      <c r="F125" s="10" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A126" s="9"/>
+      <c r="A126" s="11"/>
       <c r="B126" s="2" t="s">
         <v>81</v>
       </c>
       <c r="C126" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D126" s="11"/>
-      <c r="E126" s="9"/>
-      <c r="F126" s="14"/>
+      <c r="D126" s="12"/>
+      <c r="E126" s="11"/>
+      <c r="F126" s="10"/>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A127" s="3" t="s">
@@ -2458,7 +2458,7 @@
       <c r="E127" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="F127" s="13" t="s">
+      <c r="F127" s="9" t="s">
         <v>88</v>
       </c>
     </row>
@@ -2478,7 +2478,7 @@
       <c r="E128" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="F128" s="13" t="s">
+      <c r="F128" s="9" t="s">
         <v>88</v>
       </c>
     </row>
@@ -2498,97 +2498,6 @@
     </row>
   </sheetData>
   <mergeCells count="100">
-    <mergeCell ref="F105:F106"/>
-    <mergeCell ref="F111:F112"/>
-    <mergeCell ref="F119:F120"/>
-    <mergeCell ref="F125:F126"/>
-    <mergeCell ref="F78:F79"/>
-    <mergeCell ref="F84:F85"/>
-    <mergeCell ref="F91:F92"/>
-    <mergeCell ref="F97:F98"/>
-    <mergeCell ref="F42:F43"/>
-    <mergeCell ref="F52:F53"/>
-    <mergeCell ref="F58:F59"/>
-    <mergeCell ref="F66:F67"/>
-    <mergeCell ref="F72:F73"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="F36:F37"/>
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="C58:C59"/>
-    <mergeCell ref="D58:D59"/>
-    <mergeCell ref="A51:D51"/>
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="D52:D53"/>
-    <mergeCell ref="A57:D57"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="A41:D41"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="A35:D35"/>
-    <mergeCell ref="A24:E24"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="A18:E18"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A12:E12"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="A65:E65"/>
-    <mergeCell ref="A66:A67"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="D66:D67"/>
-    <mergeCell ref="E66:E67"/>
-    <mergeCell ref="A71:E71"/>
-    <mergeCell ref="A72:A73"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="D72:D73"/>
-    <mergeCell ref="E72:E73"/>
-    <mergeCell ref="A77:E77"/>
-    <mergeCell ref="A78:A79"/>
-    <mergeCell ref="B78:C78"/>
-    <mergeCell ref="D78:D79"/>
-    <mergeCell ref="E78:E79"/>
-    <mergeCell ref="A83:E83"/>
-    <mergeCell ref="A84:A85"/>
-    <mergeCell ref="B84:C84"/>
-    <mergeCell ref="D84:D85"/>
-    <mergeCell ref="E84:E85"/>
-    <mergeCell ref="A90:D90"/>
-    <mergeCell ref="A91:A92"/>
-    <mergeCell ref="C91:C92"/>
-    <mergeCell ref="D91:D92"/>
-    <mergeCell ref="A96:D96"/>
-    <mergeCell ref="A97:A98"/>
-    <mergeCell ref="C97:C98"/>
-    <mergeCell ref="D97:D98"/>
-    <mergeCell ref="A104:D104"/>
-    <mergeCell ref="A105:A106"/>
-    <mergeCell ref="C105:C106"/>
-    <mergeCell ref="D105:D106"/>
-    <mergeCell ref="A110:D110"/>
-    <mergeCell ref="A111:A112"/>
-    <mergeCell ref="C111:C112"/>
-    <mergeCell ref="D111:D112"/>
-    <mergeCell ref="A118:E118"/>
     <mergeCell ref="E119:E120"/>
     <mergeCell ref="A124:E124"/>
     <mergeCell ref="B125:C125"/>
@@ -2598,6 +2507,97 @@
     <mergeCell ref="A125:A126"/>
     <mergeCell ref="D125:D126"/>
     <mergeCell ref="B119:C119"/>
+    <mergeCell ref="A110:D110"/>
+    <mergeCell ref="A111:A112"/>
+    <mergeCell ref="C111:C112"/>
+    <mergeCell ref="D111:D112"/>
+    <mergeCell ref="A118:E118"/>
+    <mergeCell ref="A97:A98"/>
+    <mergeCell ref="C97:C98"/>
+    <mergeCell ref="D97:D98"/>
+    <mergeCell ref="A104:D104"/>
+    <mergeCell ref="A105:A106"/>
+    <mergeCell ref="C105:C106"/>
+    <mergeCell ref="D105:D106"/>
+    <mergeCell ref="A90:D90"/>
+    <mergeCell ref="A91:A92"/>
+    <mergeCell ref="C91:C92"/>
+    <mergeCell ref="D91:D92"/>
+    <mergeCell ref="A96:D96"/>
+    <mergeCell ref="A83:E83"/>
+    <mergeCell ref="A84:A85"/>
+    <mergeCell ref="B84:C84"/>
+    <mergeCell ref="D84:D85"/>
+    <mergeCell ref="E84:E85"/>
+    <mergeCell ref="A77:E77"/>
+    <mergeCell ref="A78:A79"/>
+    <mergeCell ref="B78:C78"/>
+    <mergeCell ref="D78:D79"/>
+    <mergeCell ref="E78:E79"/>
+    <mergeCell ref="A71:E71"/>
+    <mergeCell ref="A72:A73"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="D72:D73"/>
+    <mergeCell ref="E72:E73"/>
+    <mergeCell ref="A65:E65"/>
+    <mergeCell ref="A66:A67"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="D66:D67"/>
+    <mergeCell ref="E66:E67"/>
+    <mergeCell ref="A12:E12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A18:E18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="A35:D35"/>
+    <mergeCell ref="A24:E24"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="A41:D41"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="C58:C59"/>
+    <mergeCell ref="D58:D59"/>
+    <mergeCell ref="A51:D51"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="A57:D57"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="F36:F37"/>
+    <mergeCell ref="F42:F43"/>
+    <mergeCell ref="F52:F53"/>
+    <mergeCell ref="F58:F59"/>
+    <mergeCell ref="F66:F67"/>
+    <mergeCell ref="F72:F73"/>
+    <mergeCell ref="F105:F106"/>
+    <mergeCell ref="F111:F112"/>
+    <mergeCell ref="F119:F120"/>
+    <mergeCell ref="F125:F126"/>
+    <mergeCell ref="F78:F79"/>
+    <mergeCell ref="F84:F85"/>
+    <mergeCell ref="F91:F92"/>
+    <mergeCell ref="F97:F98"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>